<commit_message>
Creacion de Bitacora casi lista
</commit_message>
<xml_diff>
--- a/Eventos.xlsx
+++ b/Eventos.xlsx
@@ -12,15 +12,11 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
-  <si>
-    <t>NOMBRE_TFENOMENO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
   <si>
     <t>DEFINICION_TFENOMENO</t>
   </si>
@@ -28,9 +24,6 @@
     <t>DESCRIPCION</t>
   </si>
   <si>
-    <t>EXPLOSION</t>
-  </si>
-  <si>
     <t>Explosión</t>
   </si>
   <si>
@@ -40,9 +33,6 @@
     <t>OTROS</t>
   </si>
   <si>
-    <t>EROSION</t>
-  </si>
-  <si>
     <t xml:space="preserve">La erosión es un fenómeno que se produce debido a la fuerza con que actúa el agua, al escurrir sobre la superficie terrestre; o el viento, al soplar directamente sobre el suelo; o el hielo, al desplazarse formando glaciares que trituran las rocas que están bajo ellos; o la misma fuerza de gravedad, que tiende a desplazar materiales rocosos o porciones de suelo cuesta abajo. </t>
   </si>
   <si>
@@ -58,9 +48,6 @@
     <t>Varios fenómenos asociados y/o sin definir</t>
   </si>
   <si>
-    <t>HURACAN</t>
-  </si>
-  <si>
     <t>El huracán es el más severo de los fenómenos meteorológicos conocidos como ciclones tropicales. Estos son sistemas de baja presión con actividad lluviosa y eléctrica cuyos vientos rotan antihorariamente en el hemisferio Norte. Un ciclón tropical con vientos menores o iguales a 62 km/h  es llamado depresión tropical.</t>
   </si>
   <si>
@@ -85,9 +72,6 @@
     <t>Epidemia</t>
   </si>
   <si>
-    <t>ERUPCION VOLCANICA</t>
-  </si>
-  <si>
     <t>Erupción</t>
   </si>
   <si>
@@ -97,9 +81,6 @@
     <t>Marejadas</t>
   </si>
   <si>
-    <t>ACCIDENTE AEREO</t>
-  </si>
-  <si>
     <t>Accidente aéreo</t>
   </si>
   <si>
@@ -112,9 +93,6 @@
     <t>Tsunami o maremoto</t>
   </si>
   <si>
-    <t>ACCIDENTE DE TRANSITO</t>
-  </si>
-  <si>
     <t>Colisión de vehículos</t>
   </si>
   <si>
@@ -133,9 +111,6 @@
     <t>Represamiento</t>
   </si>
   <si>
-    <t>ACCIDENTE MARITIMO</t>
-  </si>
-  <si>
     <t>Accidente maritimo</t>
   </si>
   <si>
@@ -157,9 +132,6 @@
     <t>Influenza Aviar</t>
   </si>
   <si>
-    <t>ACCIDENTE FERREO</t>
-  </si>
-  <si>
     <t>Accidente Ferreo</t>
   </si>
   <si>
@@ -187,15 +159,9 @@
     <t>COLAPSO DE BANCA</t>
   </si>
   <si>
-    <t>COPLAPSO DE BANCA</t>
-  </si>
-  <si>
     <t>COLAPSO DE DIQUE</t>
   </si>
   <si>
-    <t>COPLAPSO DE DIQUE</t>
-  </si>
-  <si>
     <t>COLAPSO DE MINA</t>
   </si>
   <si>
@@ -214,23 +180,205 @@
     <t>INTOXICACIÓN</t>
   </si>
   <si>
-    <t>DERRAME DE SUSTANCIAS PELIGROSAS</t>
-  </si>
-  <si>
     <t>MAREJADA</t>
+  </si>
+  <si>
+    <t>AVALANCHA</t>
+  </si>
+  <si>
+    <t>DESERTIFICACIÓN</t>
+  </si>
+  <si>
+    <t>DESLIZAMIENTO DE TIERRA</t>
+  </si>
+  <si>
+    <t>ERUPCIÓN VOLCÁNICA</t>
+  </si>
+  <si>
+    <t>ACCIDENTE AÉREO</t>
+  </si>
+  <si>
+    <t>ACCIDENTE DE TRÁNSITO</t>
+  </si>
+  <si>
+    <t>ACCIDENTE FÉRREO</t>
+  </si>
+  <si>
+    <t>ACCIDENTE MARÍTIMO</t>
+  </si>
+  <si>
+    <t>CABEZA DE AGUA</t>
+  </si>
+  <si>
+    <t>EROSIÓN</t>
+  </si>
+  <si>
+    <t>EXPLOSIÓN</t>
+  </si>
+  <si>
+    <t>FENÓMENO ATMOSFÉRICO</t>
+  </si>
+  <si>
+    <t>HURACÁN</t>
+  </si>
+  <si>
+    <t>FALLA GEOLÓGICA</t>
+  </si>
+  <si>
+    <t>FLUJO DE CENIZA</t>
+  </si>
+  <si>
+    <t>FLUJO DE LAVA</t>
+  </si>
+  <si>
+    <t>FLUJO DE LODO</t>
+  </si>
+  <si>
+    <t>FLUJO PIRO CLÁSTICO</t>
+  </si>
+  <si>
+    <t>FRENTE FRÍO</t>
+  </si>
+  <si>
+    <t>HELADA</t>
+  </si>
+  <si>
+    <t>INCENDIO FORESTAL</t>
+  </si>
+  <si>
+    <t>INUNDACIÓN</t>
+  </si>
+  <si>
+    <t>LAHAR</t>
+  </si>
+  <si>
+    <t>LICUEFACCIÓN</t>
+  </si>
+  <si>
+    <t>LLUVIA ÁCIDA</t>
+  </si>
+  <si>
+    <t>LLUVIA DE CENIZA</t>
+  </si>
+  <si>
+    <t>OLA DE CALOR</t>
+  </si>
+  <si>
+    <t>OLA DE FRÍO</t>
+  </si>
+  <si>
+    <t>SEQUÍA</t>
+  </si>
+  <si>
+    <t>SISMO</t>
+  </si>
+  <si>
+    <t>TERREMOTO</t>
+  </si>
+  <si>
+    <t>TORMENTA</t>
+  </si>
+  <si>
+    <t>TORMENTA DE GRANIZO</t>
+  </si>
+  <si>
+    <t>VENDAVAL</t>
+  </si>
+  <si>
+    <t>VOLCÁN</t>
+  </si>
+  <si>
+    <t>CONDICIONES CLIMÁTICAS ESPACIALES</t>
+  </si>
+  <si>
+    <t>CONDICIONES CLIMÁTICAS EXTREMAS</t>
+  </si>
+  <si>
+    <t>PANDEMIA</t>
+  </si>
+  <si>
+    <t>APAGÓN</t>
+  </si>
+  <si>
+    <t>MATERIALES PELIGROSOS HAZMATH</t>
+  </si>
+  <si>
+    <t>MATERIAL RADIOACTIVO O ENERGÍA NUCLEAR</t>
+  </si>
+  <si>
+    <t>Las condiciones climáticas espaciales extremas podrían provocar daños en infraestructuras críticas, especialmente en el sistema de suministro eléctrico, lo cual resalta la importancia de prepararse.</t>
+  </si>
+  <si>
+    <t>todo el mundo corre riesgo y debe tomar medidas para prepararse para cuando haya condiciones climáticas extremas en su área. Saber cuáles son los peligros climáticos más frecuentes en su área, su vulnerabilidad, y qué medidas puede tomar puede salvar su vida y la de otras personas.</t>
+  </si>
+  <si>
+    <t>Los problemas de deslizamientos de tierra pueden tener lugar debido a un mal manejo de la tierra, particularmente en montañas, cañones y regiones costeras. En áreas que resultaron incendiadas, un nivel menor de precipitaciones puede originar deslizamientos de tierra. La zonificación del uso de la tierra, las inspecciones profesionales y un diseño adecuado pueden minimizar la incidencia de muchos problemas de deslizamientos de tierra, corrientes de lodo y avalanchas de escombros.</t>
+  </si>
+  <si>
+    <t>TERRORISMO</t>
+  </si>
+  <si>
+    <t>ANTICICLÓN/ANTIHURACÁN</t>
+  </si>
+  <si>
+    <t>CRECIENTE SÚBITA</t>
+  </si>
+  <si>
+    <t>ACCIDENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCIDENTE MINERO </t>
+  </si>
+  <si>
+    <t>COLAPSO</t>
+  </si>
+  <si>
+    <t>CONTAMINACIÓN</t>
+  </si>
+  <si>
+    <t>DERRAME</t>
+  </si>
+  <si>
+    <t>INCENDIO ESTRUCTURAL</t>
+  </si>
+  <si>
+    <t>TORMENTA ELÉCTRICA Y DE RAYOS</t>
+  </si>
+  <si>
+    <t>Nombre de fenómeno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -253,8 +401,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,402 +713,612 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection sqref="A1:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103" customWidth="1"/>
     <col min="3" max="3" width="68.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
+      <c r="A7" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+      <c r="A10" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
+      <c r="A11" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
+      <c r="A13" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+      <c r="A14" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
         <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
+      <c r="A34" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>29</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B65" t="s">
         <v>30</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" t="s">
         <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -959,6 +1326,7 @@
     <sortCondition ref="A2:A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>